<commit_message>
Views and Stored Procedure Results
</commit_message>
<xml_diff>
--- a/Queries/ADVANDB_FernandezSanPedroSyfu_Statistics_v1.xlsx
+++ b/Queries/ADVANDB_FernandezSanPedroSyfu_Statistics_v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Query 1" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="8">
   <si>
     <t>Base</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Improvement</t>
   </si>
 </sst>
 </file>
@@ -368,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -413,8 +416,14 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -452,8 +461,16 @@
         <f>AVERAGE(B2:K2)</f>
         <v>129.9453</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2</f>
+        <v>129.9453</v>
+      </c>
+      <c r="N2">
+        <f>(L2-M2) * 100/M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -491,30 +508,62 @@
         <f>AVERAGE(B3:K3)</f>
         <v>133.93289999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2</f>
+        <v>129.9453</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">(L3-M3) * 100/M3</f>
+        <v>3.0686758197487607</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="L4" t="e">
-        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:K4)</f>
+        <f t="shared" ref="L4:L6" si="1">AVERAGE(B4:K4)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" ref="M4:M6" si="2">M3</f>
+        <v>129.9453</v>
+      </c>
+      <c r="N4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="L5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>129.9453</v>
+      </c>
+      <c r="N5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="L6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>129.9453</v>
+      </c>
+      <c r="N6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -526,10 +575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +586,7 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -574,8 +623,14 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -613,8 +668,16 @@
         <f>AVERAGE(B2:K2)</f>
         <v>13.709299999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2</f>
+        <v>13.709299999999999</v>
+      </c>
+      <c r="N2">
+        <f>(M2-L2) * 100/M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -652,8 +715,16 @@
         <f>AVERAGE(B3:K3)</f>
         <v>12.943699999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2</f>
+        <v>13.709299999999999</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">(M3-L3) * 100/M3</f>
+        <v>5.5845302094198894</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -688,26 +759,110 @@
         <v>1.6E-2</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:K4)</f>
+        <f t="shared" ref="L4:L6" si="1">AVERAGE(B4:K4)</f>
         <v>7.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f>M3</f>
+        <v>13.709299999999999</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>99.943833747893763</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" t="e">
+      <c r="B5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="M5">
+        <f>M4</f>
+        <v>13.709299999999999</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>99.932162838365201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="e">
+      <c r="B6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>1.11E-2</v>
+      </c>
+      <c r="M6">
+        <f>M5</f>
+        <v>13.709299999999999</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>99.919033065145541</v>
       </c>
     </row>
   </sheetData>
@@ -717,10 +872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +883,7 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -765,8 +920,14 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -804,8 +965,16 @@
         <f>AVERAGE(B2:K2)</f>
         <v>5.9594000000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2</f>
+        <v>5.9594000000000005</v>
+      </c>
+      <c r="N2">
+        <f>(M2-L2) * 100/M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -843,62 +1012,154 @@
         <f>AVERAGE(B3:K3)</f>
         <v>5.6201999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2</f>
+        <v>5.9594000000000005</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">(M3-L3) * 100/M3</f>
+        <v>5.6918481726348436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.6719999999999997</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C4">
-        <v>5.6719999999999997</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>5.6719999999999997</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E4">
-        <v>5.5780000000000003</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>5.64</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>5.5149999999999997</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>5.5309999999999997</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>5.4379999999999997</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>5.593</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>5.657</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:K4)</f>
-        <v>5.5967999999999991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L4:L6" si="1">AVERAGE(B4:K4)</f>
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M6" si="2">M3</f>
+        <v>5.9594000000000005</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>99.947981340403402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" t="e">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000004E-3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>5.9594000000000005</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>99.919454978689132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="e">
+      <c r="B6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>5.9594000000000005</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>99.843944021210206</v>
       </c>
     </row>
   </sheetData>
@@ -908,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +1180,7 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -956,8 +1217,14 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -995,8 +1262,16 @@
         <f>AVERAGE(B2:K2)</f>
         <v>0.53420000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2</f>
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="N2">
+        <f>(M2-L2) * 100/M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1034,8 +1309,16 @@
         <f>AVERAGE(B3:K3)</f>
         <v>0.15160000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2</f>
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">(M3-L3) * 100/M3</f>
+        <v>71.621115687008611</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1070,26 +1353,110 @@
         <v>1.6E-2</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:K4)</f>
+        <f t="shared" ref="L4:L6" si="1">AVERAGE(B4:K4)</f>
         <v>1.2500000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" ref="M4:M6" si="2">M3</f>
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>97.660052414825913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" t="e">
+      <c r="B5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>97.978285286409573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="e">
+      <c r="B6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>1.4100000000000001E-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>97.360539123923616</v>
       </c>
     </row>
   </sheetData>
@@ -1099,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1477,7 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1147,8 +1514,14 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1186,8 +1559,16 @@
         <f>AVERAGE(B2:K2)</f>
         <v>14.714099999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2</f>
+        <v>14.714099999999998</v>
+      </c>
+      <c r="N2">
+        <f>(M2-L2)* 100/M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1225,8 +1606,16 @@
         <f>AVERAGE(B3:K3)</f>
         <v>14.533199999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2</f>
+        <v>14.714099999999998</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">(M3-L3)* 100/M3</f>
+        <v>1.229432992843595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1261,26 +1650,110 @@
         <v>13.218999999999999</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:K4)</f>
+        <f t="shared" ref="L4:L6" si="1">AVERAGE(B4:K4)</f>
         <v>13.378</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" ref="M4:M6" si="2">M3</f>
+        <v>14.714099999999998</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>9.0804058692002805</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" t="e">
+      <c r="B5">
+        <v>13.468999999999999</v>
+      </c>
+      <c r="C5">
+        <v>13.406000000000001</v>
+      </c>
+      <c r="D5">
+        <v>13.657</v>
+      </c>
+      <c r="E5">
+        <v>13.218999999999999</v>
+      </c>
+      <c r="F5">
+        <v>13.25</v>
+      </c>
+      <c r="G5">
+        <v>13.436999999999999</v>
+      </c>
+      <c r="H5">
+        <v>13.25</v>
+      </c>
+      <c r="I5">
+        <v>13.202999999999999</v>
+      </c>
+      <c r="J5">
+        <v>13.281000000000001</v>
+      </c>
+      <c r="K5">
+        <v>13.172000000000001</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>13.334400000000002</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>14.714099999999998</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>9.3767202887026482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="e">
+      <c r="B6">
+        <v>13.281000000000001</v>
+      </c>
+      <c r="C6">
+        <v>13.61</v>
+      </c>
+      <c r="D6">
+        <v>13.563000000000001</v>
+      </c>
+      <c r="E6">
+        <v>13.484999999999999</v>
+      </c>
+      <c r="F6">
+        <v>13.577999999999999</v>
+      </c>
+      <c r="G6">
+        <v>13.922000000000001</v>
+      </c>
+      <c r="H6">
+        <v>13.484</v>
+      </c>
+      <c r="I6">
+        <v>13.516</v>
+      </c>
+      <c r="J6">
+        <v>13.327999999999999</v>
+      </c>
+      <c r="K6">
+        <v>13.436999999999999</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>13.5204</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>14.714099999999998</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>8.1126266642200218</v>
       </c>
     </row>
   </sheetData>
@@ -1290,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1774,7 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1338,8 +1811,14 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1377,8 +1856,16 @@
         <f>AVERAGE(B2:K2)</f>
         <v>0.18450000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2</f>
+        <v>0.18450000000000003</v>
+      </c>
+      <c r="N2">
+        <f>(M2-L2)*100/M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1416,8 +1903,16 @@
         <f>AVERAGE(B3:K3)</f>
         <v>7.9699999999999993E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2</f>
+        <v>0.18450000000000003</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">(M3-L3)*100/M3</f>
+        <v>56.802168021680231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1452,26 +1947,110 @@
         <v>1.6E-2</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:K4)</f>
+        <f t="shared" ref="L4:L6" si="1">AVERAGE(B4:K4)</f>
         <v>1.0999999999999999E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" ref="M4:M6" si="2">M3</f>
+        <v>0.18450000000000003</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>94.037940379403793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" t="e">
+      <c r="B5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>1.09E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0.18450000000000003</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>94.092140921409211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="e">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0.18450000000000003</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>95.77235772357723</v>
       </c>
     </row>
   </sheetData>
@@ -1481,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +2071,7 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1529,8 +2108,14 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1568,8 +2153,16 @@
         <f>AVERAGE(B2:K2)</f>
         <v>0.1263</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>L2</f>
+        <v>0.1263</v>
+      </c>
+      <c r="N2">
+        <f>(M2-L2)*100/M2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1607,52 +2200,68 @@
         <f>AVERAGE(B3:K3)</f>
         <v>0.1341</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>M2</f>
+        <v>0.1263</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">(M3-L3)*100/M3</f>
+        <v>-6.1757719714964381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.14099999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="C4">
+        <v>0.156</v>
+      </c>
+      <c r="D4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E4">
         <v>0.125</v>
       </c>
-      <c r="D4">
-        <v>0.125</v>
-      </c>
-      <c r="E4">
-        <v>0.28199999999999997</v>
-      </c>
       <c r="F4">
-        <v>0.14000000000000001</v>
+        <v>0.157</v>
       </c>
       <c r="G4">
         <v>0.156</v>
       </c>
       <c r="H4">
-        <v>0.125</v>
+        <v>0.156</v>
       </c>
       <c r="I4">
-        <v>0.14000000000000001</v>
+        <v>0.109</v>
       </c>
       <c r="J4">
         <v>0.17199999999999999</v>
       </c>
       <c r="K4">
-        <v>0.20300000000000001</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:K4)</f>
-        <v>0.16089999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L4:L6" si="1">AVERAGE(B4:K4)</f>
+        <v>0.14219999999999999</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M6" si="2">M3</f>
+        <v>0.1263</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>-12.589073634204276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.14099999999999999</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="C5">
         <v>0.156</v>
@@ -1661,38 +2270,84 @@
         <v>0.156</v>
       </c>
       <c r="E5">
-        <v>0.188</v>
+        <v>0.187</v>
       </c>
       <c r="F5">
-        <v>6.3E-2</v>
+        <v>0.157</v>
       </c>
       <c r="G5">
-        <v>7.8E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H5">
-        <v>0.125</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="I5">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="J5">
         <v>0.156</v>
       </c>
-      <c r="J5">
-        <v>0.14000000000000001</v>
-      </c>
       <c r="K5">
-        <v>0.14000000000000001</v>
+        <v>0.157</v>
       </c>
       <c r="L5">
+        <f t="shared" si="1"/>
+        <v>0.1656</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0.1263</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="0"/>
-        <v>0.1343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-31.11638954869359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="e">
+      <c r="B6">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="D6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.125</v>
+      </c>
+      <c r="F6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.109</v>
+      </c>
+      <c r="I6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="J6">
+        <v>7.8E-2</v>
+      </c>
+      <c r="K6">
+        <v>0.125</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>0.1172</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0.1263</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>7.2050673000791745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>